<commit_message>
Added more functions to dataCleaner script
</commit_message>
<xml_diff>
--- a/HabitatProject/ProjectSchedule.xlsx
+++ b/HabitatProject/ProjectSchedule.xlsx
@@ -1529,9 +1529,6 @@
     <t>Evaluate georeferencing necessity</t>
   </si>
   <si>
-    <t>Clean up data in Excel, save in DB</t>
-  </si>
-  <si>
     <t>Retrieve &amp; Evaluate dataset</t>
   </si>
   <si>
@@ -1581,6 +1578,9 @@
   </si>
   <si>
     <t>Document results</t>
+  </si>
+  <si>
+    <t>Clean up data</t>
   </si>
 </sst>
 </file>
@@ -2934,6 +2934,24 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2941,27 +2959,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3013,7 +3013,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="38">
     <dxf>
       <border>
         <left style="thin">
@@ -3025,32 +3025,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3374,266 +3348,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3745,7 +3459,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3850,7 +3564,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3934,7 +3648,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3989,7 +3703,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4044,7 +3758,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4372,8 +4086,8 @@
   <dimension ref="A1:BN51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4401,29 +4115,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="169" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="169"/>
+      <c r="AC1" s="169"/>
+      <c r="AD1" s="169"/>
+      <c r="AE1" s="169"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52"/>
@@ -4466,11 +4180,11 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="171">
         <v>43313</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4480,180 +4194,180 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="163" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="164"/>
+      <c r="P4" s="164"/>
+      <c r="Q4" s="165"/>
+      <c r="R4" s="163" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
+      <c r="S4" s="164"/>
+      <c r="T4" s="164"/>
+      <c r="U4" s="164"/>
+      <c r="V4" s="164"/>
+      <c r="W4" s="164"/>
+      <c r="X4" s="165"/>
+      <c r="Y4" s="163" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
+      <c r="Z4" s="164"/>
+      <c r="AA4" s="164"/>
+      <c r="AB4" s="164"/>
+      <c r="AC4" s="164"/>
+      <c r="AD4" s="164"/>
+      <c r="AE4" s="165"/>
+      <c r="AF4" s="163" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
+      <c r="AG4" s="164"/>
+      <c r="AH4" s="164"/>
+      <c r="AI4" s="164"/>
+      <c r="AJ4" s="164"/>
+      <c r="AK4" s="164"/>
+      <c r="AL4" s="165"/>
+      <c r="AM4" s="163" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
+      <c r="AN4" s="164"/>
+      <c r="AO4" s="164"/>
+      <c r="AP4" s="164"/>
+      <c r="AQ4" s="164"/>
+      <c r="AR4" s="164"/>
+      <c r="AS4" s="165"/>
+      <c r="AT4" s="163" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
+      <c r="AU4" s="164"/>
+      <c r="AV4" s="164"/>
+      <c r="AW4" s="164"/>
+      <c r="AX4" s="164"/>
+      <c r="AY4" s="164"/>
+      <c r="AZ4" s="165"/>
+      <c r="BA4" s="163" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
+      <c r="BB4" s="164"/>
+      <c r="BC4" s="164"/>
+      <c r="BD4" s="164"/>
+      <c r="BE4" s="164"/>
+      <c r="BF4" s="164"/>
+      <c r="BG4" s="165"/>
+      <c r="BH4" s="163" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
+      <c r="BI4" s="164"/>
+      <c r="BJ4" s="164"/>
+      <c r="BK4" s="164"/>
+      <c r="BL4" s="164"/>
+      <c r="BM4" s="164"/>
+      <c r="BN4" s="165"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="169">
+      <c r="K5" s="166">
         <f>K6</f>
         <v>43311</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="166">
         <f>R6</f>
         <v>43318</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="167"/>
+      <c r="V5" s="167"/>
+      <c r="W5" s="167"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="166">
         <f>Y6</f>
         <v>43325</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="167"/>
+      <c r="AC5" s="167"/>
+      <c r="AD5" s="167"/>
+      <c r="AE5" s="168"/>
+      <c r="AF5" s="166">
         <f>AF6</f>
         <v>43332</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
+      <c r="AG5" s="167"/>
+      <c r="AH5" s="167"/>
+      <c r="AI5" s="167"/>
+      <c r="AJ5" s="167"/>
+      <c r="AK5" s="167"/>
+      <c r="AL5" s="168"/>
+      <c r="AM5" s="166">
         <f>AM6</f>
         <v>43339</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
+      <c r="AN5" s="167"/>
+      <c r="AO5" s="167"/>
+      <c r="AP5" s="167"/>
+      <c r="AQ5" s="167"/>
+      <c r="AR5" s="167"/>
+      <c r="AS5" s="168"/>
+      <c r="AT5" s="166">
         <f>AT6</f>
         <v>43346</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
+      <c r="AU5" s="167"/>
+      <c r="AV5" s="167"/>
+      <c r="AW5" s="167"/>
+      <c r="AX5" s="167"/>
+      <c r="AY5" s="167"/>
+      <c r="AZ5" s="168"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>43353</v>
       </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
+      <c r="BB5" s="167"/>
+      <c r="BC5" s="167"/>
+      <c r="BD5" s="167"/>
+      <c r="BE5" s="167"/>
+      <c r="BF5" s="167"/>
+      <c r="BG5" s="168"/>
+      <c r="BH5" s="166">
         <f>BH6</f>
         <v>43360</v>
       </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
+      <c r="BI5" s="167"/>
+      <c r="BJ5" s="167"/>
+      <c r="BK5" s="167"/>
+      <c r="BL5" s="167"/>
+      <c r="BM5" s="167"/>
+      <c r="BN5" s="168"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -5244,7 +4958,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="64">
         <f t="shared" ref="I9" si="6">IF(OR(F9=0,E9=0)," - ",NETWORKDAYS(E9,F9))</f>
@@ -5328,7 +5042,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="64">
         <f t="shared" si="4"/>
@@ -5397,7 +5111,7 @@
         <v>1.2</v>
       </c>
       <c r="B11" s="126" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="127"/>
       <c r="E11" s="100">
@@ -5410,7 +5124,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I11" s="64">
         <v>1</v>
@@ -5473,13 +5187,13 @@
       <c r="BM11" s="107"/>
       <c r="BN11" s="107"/>
     </row>
-    <row r="12" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.1</v>
       </c>
       <c r="B12" s="128" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="D12" s="127"/>
       <c r="E12" s="100">
@@ -5493,7 +5207,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="63">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I12" s="64">
         <f t="shared" ref="I12" si="8">IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
@@ -5577,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="64">
         <f t="shared" ref="I13" si="10">IF(OR(F13=0,E13=0)," - ",NETWORKDAYS(E13,F13))</f>
@@ -5661,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="64">
         <f t="shared" ref="I14" si="12">IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
@@ -5731,7 +5445,7 @@
         <v>1.3</v>
       </c>
       <c r="B15" s="126" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" s="127"/>
       <c r="E15" s="100">
@@ -5815,7 +5529,7 @@
         <v>1.3.1</v>
       </c>
       <c r="B16" s="128" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="127"/>
       <c r="E16" s="100">
@@ -5899,7 +5613,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B17" s="128" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="127"/>
       <c r="E17" s="100">
@@ -5983,7 +5697,7 @@
         <v>1.4</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="127"/>
       <c r="E18" s="100">
@@ -6067,7 +5781,7 @@
         <v>1.4.1</v>
       </c>
       <c r="B19" s="128" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="127"/>
       <c r="E19" s="100">
@@ -6151,7 +5865,7 @@
         <v>1.4.2</v>
       </c>
       <c r="B20" s="128" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="127"/>
       <c r="E20" s="100">
@@ -6235,7 +5949,7 @@
         <v>1.5</v>
       </c>
       <c r="B21" s="126" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D21" s="127"/>
       <c r="E21" s="100">
@@ -6319,7 +6033,7 @@
         <v>1.5.1</v>
       </c>
       <c r="B22" s="128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D22" s="127"/>
       <c r="E22" s="100">
@@ -6403,7 +6117,7 @@
         <v>1.5.2</v>
       </c>
       <c r="B23" s="128" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" s="127"/>
       <c r="E23" s="100">
@@ -6487,7 +6201,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D24" s="56"/>
       <c r="E24" s="102"/>
@@ -6561,11 +6275,11 @@
     </row>
     <row r="25" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A25:A30" si="22">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B25" s="126" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="100">
@@ -6645,11 +6359,11 @@
     </row>
     <row r="26" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="22"/>
         <v>2.2</v>
       </c>
       <c r="B26" s="126" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26" s="127"/>
       <c r="E26" s="100">
@@ -6729,11 +6443,11 @@
     </row>
     <row r="27" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="22"/>
         <v>2.3</v>
       </c>
       <c r="B27" s="126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="100">
@@ -6813,11 +6527,11 @@
     </row>
     <row r="28" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="22"/>
         <v>2.4</v>
       </c>
       <c r="B28" s="126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D28" s="127"/>
       <c r="E28" s="100">
@@ -6897,11 +6611,11 @@
     </row>
     <row r="29" spans="1:66" s="61" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="22"/>
         <v>2.5</v>
       </c>
       <c r="B29" s="126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" s="127"/>
       <c r="E29" s="100">
@@ -6981,18 +6695,18 @@
     </row>
     <row r="30" spans="1:66" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="22"/>
         <v>2.6</v>
       </c>
       <c r="B30" s="126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D30" s="127"/>
       <c r="E30" s="100">
         <v>43354</v>
       </c>
       <c r="F30" s="101">
-        <f t="shared" ref="F30" si="22">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
+        <f t="shared" ref="F30" si="23">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
         <v>43356</v>
       </c>
       <c r="G30" s="62">
@@ -7002,7 +6716,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="64">
-        <f t="shared" ref="I30" si="23">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
+        <f t="shared" ref="I30" si="24">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
         <v>3</v>
       </c>
       <c r="J30" s="95"/>
@@ -8353,7 +8067,7 @@
       <c r="D47" s="79"/>
       <c r="E47" s="100"/>
       <c r="F47" s="101" t="str">
-        <f t="shared" ref="F47:F50" si="24">IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
+        <f t="shared" ref="F47:F50" si="25">IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G47" s="62"/>
@@ -8432,13 +8146,13 @@
       <c r="D48" s="79"/>
       <c r="E48" s="100"/>
       <c r="F48" s="101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G48" s="62"/>
       <c r="H48" s="63"/>
       <c r="I48" s="80" t="str">
-        <f t="shared" ref="I48:I50" si="25">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
+        <f t="shared" ref="I48:I50" si="26">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J48" s="99"/>
@@ -8511,13 +8225,13 @@
       <c r="D49" s="79"/>
       <c r="E49" s="100"/>
       <c r="F49" s="101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G49" s="62"/>
       <c r="H49" s="63"/>
       <c r="I49" s="80" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J49" s="99"/>
@@ -8590,13 +8304,13 @@
       <c r="D50" s="79"/>
       <c r="E50" s="100"/>
       <c r="F50" s="101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G50" s="62"/>
       <c r="H50" s="63"/>
       <c r="I50" s="80" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J50" s="99"/>
@@ -8728,6 +8442,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8738,15 +8461,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8 H18 H10:H11 H21 H24:H29 H31:H50">
@@ -8764,20 +8478,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="40" priority="97">
+    <cfRule type="expression" dxfId="37" priority="97">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN8 K10:BN11 K17:BN18 K21:BN21 K24:BN29 K31:BN50">
-    <cfRule type="expression" dxfId="39" priority="100">
+    <cfRule type="expression" dxfId="36" priority="100">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="101">
+    <cfRule type="expression" dxfId="35" priority="101">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN8 K18:BN18 K10:BN11 K21:BN21 K24:BN29 K31:BN50">
-    <cfRule type="expression" dxfId="37" priority="60">
+    <cfRule type="expression" dxfId="34" priority="60">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8824,15 +8538,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="36" priority="51">
+    <cfRule type="expression" dxfId="33" priority="51">
       <formula>AND($E15&lt;=K$6,ROUNDDOWN(($F15-$E15+1)*$H15,0)+$E15-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="52">
+    <cfRule type="expression" dxfId="32" priority="52">
       <formula>AND(NOT(ISBLANK($E15)),$E15&lt;=K$6,$F15&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="34" priority="50">
+    <cfRule type="expression" dxfId="31" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8851,15 +8565,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="33" priority="47">
+    <cfRule type="expression" dxfId="30" priority="47">
       <formula>AND($E13&lt;=K$6,ROUNDDOWN(($F13-$E13+1)*$H13,0)+$E13-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="48">
+    <cfRule type="expression" dxfId="29" priority="48">
       <formula>AND(NOT(ISBLANK($E13)),$E13&lt;=K$6,$F13&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="31" priority="46">
+    <cfRule type="expression" dxfId="28" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8878,28 +8592,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:BN9">
-    <cfRule type="expression" dxfId="30" priority="43">
+    <cfRule type="expression" dxfId="27" priority="43">
       <formula>AND($E9&lt;=K$6,ROUNDDOWN(($F9-$E9+1)*$H9,0)+$E9-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="44">
+    <cfRule type="expression" dxfId="26" priority="44">
       <formula>AND(NOT(ISBLANK($E9)),$E9&lt;=K$6,$F9&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:BN9">
-    <cfRule type="expression" dxfId="28" priority="42">
+    <cfRule type="expression" dxfId="25" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="27" priority="39">
+    <cfRule type="expression" dxfId="24" priority="39">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="40">
+    <cfRule type="expression" dxfId="23" priority="40">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="25" priority="38">
+    <cfRule type="expression" dxfId="22" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8918,28 +8632,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>AND($E12&lt;=K$6,ROUNDDOWN(($F12-$E12+1)*$H12,0)+$E12-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="36">
+    <cfRule type="expression" dxfId="20" priority="36">
       <formula>AND(NOT(ISBLANK($E12)),$E12&lt;=K$6,$F12&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="22" priority="34">
+    <cfRule type="expression" dxfId="19" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:BN17">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>AND($E16&lt;=K$6,ROUNDDOWN(($F16-$E16+1)*$H16,0)+$E16-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>AND(NOT(ISBLANK($E16)),$E16&lt;=K$6,$F16&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8958,15 +8672,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="15" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>AND($E19&lt;=K$6,ROUNDDOWN(($F19-$E19+1)*$H19,0)+$E19-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>AND(NOT(ISBLANK($E19)),$E19&lt;=K$6,$F19&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8985,15 +8699,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>AND($E20&lt;=K$6,ROUNDDOWN(($F20-$E20+1)*$H20,0)+$E20-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="10" priority="16">
       <formula>AND(NOT(ISBLANK($E20)),$E20&lt;=K$6,$F20&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9012,7 +8726,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="9" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9031,15 +8745,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>AND($E22&lt;=K$6,ROUNDDOWN(($F22-$E22+1)*$H22,0)+$E22-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>AND(NOT(ISBLANK($E22)),$E22&lt;=K$6,$F22&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9058,15 +8772,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9085,15 +8799,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($E30&lt;=K$6,ROUNDDOWN(($F30-$E30+1)*$H30,0)+$E30-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND(NOT(ISBLANK($E30)),$E30&lt;=K$6,$F30&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed encoding issue with outputGeolocateCSV function
</commit_message>
<xml_diff>
--- a/HabitatProject/ProjectSchedule.xlsx
+++ b/HabitatProject/ProjectSchedule.xlsx
@@ -2934,24 +2934,6 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2959,9 +2941,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3013,7 +3013,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="28">
     <dxf>
       <border>
         <left style="thin">
@@ -3025,20 +3025,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -3053,18 +3039,16 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -3079,20 +3063,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -3103,46 +3073,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -3459,7 +3389,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3564,7 +3494,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3648,7 +3578,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3703,7 +3633,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3758,7 +3688,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4087,7 +4017,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4115,29 +4045,29 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="132"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52"/>
@@ -4180,11 +4110,11 @@
       <c r="B4" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="168">
         <v>43313</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="111"/>
       <c r="G4" s="114" t="s">
         <v>75</v>
@@ -4194,180 +4124,180 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="110"/>
       <c r="B5" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="166">
+      <c r="K5" s="169">
         <f>K6</f>
         <v>43311</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
+      <c r="L5" s="170"/>
+      <c r="M5" s="170"/>
+      <c r="N5" s="170"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="169">
         <f>R6</f>
         <v>43318</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="169">
         <f>Y6</f>
         <v>43325</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>43332</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="169">
         <f>AM6</f>
         <v>43339</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="171"/>
+      <c r="AT5" s="169">
         <f>AT6</f>
         <v>43346</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
+      <c r="AX5" s="170"/>
+      <c r="AY5" s="170"/>
+      <c r="AZ5" s="171"/>
+      <c r="BA5" s="169">
         <f>BA6</f>
         <v>43353</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
+      <c r="BB5" s="170"/>
+      <c r="BC5" s="170"/>
+      <c r="BD5" s="170"/>
+      <c r="BE5" s="170"/>
+      <c r="BF5" s="170"/>
+      <c r="BG5" s="171"/>
+      <c r="BH5" s="169">
         <f>BH6</f>
         <v>43360</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
+      <c r="BI5" s="170"/>
+      <c r="BJ5" s="170"/>
+      <c r="BK5" s="170"/>
+      <c r="BL5" s="170"/>
+      <c r="BM5" s="170"/>
+      <c r="BN5" s="171"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -5124,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="63">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="I11" s="64">
         <v>1</v>
@@ -5207,7 +5137,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="63">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="I12" s="64">
         <f t="shared" ref="I12" si="8">IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
@@ -5459,7 +5389,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="63">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I15" s="64">
         <f t="shared" ref="I15:I16" si="14">IF(OR(F15=0,E15=0)," - ",NETWORKDAYS(E15,F15))</f>
@@ -5543,7 +5473,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="64">
         <f t="shared" si="14"/>
@@ -5627,7 +5557,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="63">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="64">
         <f t="shared" ref="I17" si="16">IF(OR(F17=0,E17=0)," - ",NETWORKDAYS(E17,F17))</f>
@@ -8442,15 +8372,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8461,10 +8382,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8 H18 H10:H11 H21 H24:H29 H31:H50">
-    <cfRule type="dataBar" priority="54">
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8478,25 +8408,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="37" priority="97">
+    <cfRule type="expression" dxfId="27" priority="101">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN8 K10:BN11 K17:BN18 K21:BN21 K24:BN29 K31:BN50">
-    <cfRule type="expression" dxfId="36" priority="100">
+  <conditionalFormatting sqref="K8:BN8 K10:BN11 K17:BN50">
+    <cfRule type="expression" dxfId="26" priority="104">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="101">
+    <cfRule type="expression" dxfId="25" priority="105">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN8 K18:BN18 K10:BN11 K21:BN21 K24:BN29 K31:BN50">
-    <cfRule type="expression" dxfId="34" priority="60">
+    <cfRule type="expression" dxfId="24" priority="64">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8510,7 +8440,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="dataBar" priority="45">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8524,7 +8454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8538,20 +8468,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="33" priority="51">
+    <cfRule type="expression" dxfId="23" priority="55">
       <formula>AND($E15&lt;=K$6,ROUNDDOWN(($F15-$E15+1)*$H15,0)+$E15-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="22" priority="56">
       <formula>AND(NOT(ISBLANK($E15)),$E15&lt;=K$6,$F15&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="31" priority="50">
+    <cfRule type="expression" dxfId="21" priority="54">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8565,20 +8495,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="30" priority="47">
+    <cfRule type="expression" dxfId="20" priority="51">
       <formula>AND($E13&lt;=K$6,ROUNDDOWN(($F13-$E13+1)*$H13,0)+$E13-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="48">
+    <cfRule type="expression" dxfId="19" priority="52">
       <formula>AND(NOT(ISBLANK($E13)),$E13&lt;=K$6,$F13&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="28" priority="46">
+    <cfRule type="expression" dxfId="18" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="dataBar" priority="33">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8592,33 +8522,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:BN9">
-    <cfRule type="expression" dxfId="27" priority="43">
+    <cfRule type="expression" dxfId="17" priority="47">
       <formula>AND($E9&lt;=K$6,ROUNDDOWN(($F9-$E9+1)*$H9,0)+$E9-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="44">
+    <cfRule type="expression" dxfId="16" priority="48">
       <formula>AND(NOT(ISBLANK($E9)),$E9&lt;=K$6,$F9&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:BN9">
-    <cfRule type="expression" dxfId="25" priority="42">
+    <cfRule type="expression" dxfId="15" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="24" priority="39">
+    <cfRule type="expression" dxfId="14" priority="43">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="40">
+    <cfRule type="expression" dxfId="13" priority="44">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="22" priority="38">
+    <cfRule type="expression" dxfId="12" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8632,33 +8562,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="21" priority="35">
+    <cfRule type="expression" dxfId="11" priority="39">
       <formula>AND($E12&lt;=K$6,ROUNDDOWN(($F12-$E12+1)*$H12,0)+$E12-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36">
+    <cfRule type="expression" dxfId="10" priority="40">
       <formula>AND(NOT(ISBLANK($E12)),$E12&lt;=K$6,$F12&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="19" priority="34">
+    <cfRule type="expression" dxfId="9" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:BN17">
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="8" priority="30">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="7" priority="27">
       <formula>AND($E16&lt;=K$6,ROUNDDOWN(($F16-$E16+1)*$H16,0)+$E16-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="6" priority="28">
       <formula>AND(NOT(ISBLANK($E16)),$E16&lt;=K$6,$F16&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8672,20 +8602,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="5" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="14" priority="19">
-      <formula>AND($E19&lt;=K$6,ROUNDDOWN(($F19-$E19+1)*$H19,0)+$E19-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="20">
-      <formula>AND(NOT(ISBLANK($E19)),$E19&lt;=K$6,$F19&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8699,20 +8621,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="12" priority="18">
+    <cfRule type="expression" dxfId="4" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>AND($E20&lt;=K$6,ROUNDDOWN(($F20-$E20+1)*$H20,0)+$E20-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="16">
-      <formula>AND(NOT(ISBLANK($E20)),$E20&lt;=K$6,$F20&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8726,12 +8640,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="9" priority="14">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8745,20 +8659,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>AND($E22&lt;=K$6,ROUNDDOWN(($F22-$E22+1)*$H22,0)+$E22-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12">
-      <formula>AND(NOT(ISBLANK($E22)),$E22&lt;=K$6,$F22&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="2" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8772,20 +8678,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8799,15 +8697,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND($E30&lt;=K$6,ROUNDDOWN(($F30-$E30+1)*$H30,0)+$E30-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>AND(NOT(ISBLANK($E30)),$E30&lt;=K$6,$F30&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>